<commit_message>
AssembleReference,  AnalyzeBAMs, and VCF R script updates, and added ReferenceBased script
AssembleReference now runs bbduk twice, to trim each read end while retaining PE info, and K trims from a provided ISSR motif fasta. AnalyzeBAMs now works properly with the samples file. The VCF script conducts several analysis types, but still has not been configured as part of the pipeline -- variables for paths and file names need to be generalized. ReferenceBased is an alternative to AssembleReference, where a reference genome is provided and the reads are trimmed and the directory structure expected by downstream analyses is setup.
</commit_message>
<xml_diff>
--- a/development notes/development_run_results.xlsx
+++ b/development notes/development_run_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Documents\ISSRseq\development notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BBFBB6-156C-4918-9F64-DCF9686FB0DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA99404-CAEB-4C2D-BBF7-5F02BF119CEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="2490" windowWidth="22800" windowHeight="10860" xr2:uid="{99C3184B-795E-4B96-8633-BF33F0E94C1E}"/>
+    <workbookView xWindow="3945" yWindow="5760" windowWidth="23310" windowHeight="8355" xr2:uid="{99C3184B-795E-4B96-8633-BF33F0E94C1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Taxon</t>
   </si>
@@ -54,9 +54,6 @@
     <t>pooled PCRs, sheared</t>
   </si>
   <si>
-    <t>GATK-filtered SNPs</t>
-  </si>
-  <si>
     <t>variants called</t>
   </si>
   <si>
@@ -109,6 +106,21 @@
   </si>
   <si>
     <t>STACKS -- myco run -- SE</t>
+  </si>
+  <si>
+    <t>C. bentleyi, involuta, and striata</t>
+  </si>
+  <si>
+    <t>2,721 (250 bp min)</t>
+  </si>
+  <si>
+    <t>found in all individuals</t>
+  </si>
+  <si>
+    <t>found in 90% of individuals</t>
+  </si>
+  <si>
+    <t>filtered SNPs</t>
   </si>
 </sst>
 </file>
@@ -480,15 +492,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DFE0D0-A0D4-41B8-9114-A09382CB63CC}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
@@ -496,51 +508,58 @@
     <col min="6" max="6" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="25.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" s="2">
         <v>122941</v>
@@ -551,22 +570,28 @@
       <c r="H2" s="1">
         <v>504</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1">
+        <v>138</v>
+      </c>
+      <c r="J2" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="2">
         <v>1064221</v>
@@ -577,129 +602,179 @@
       <c r="H3" s="2">
         <v>6497</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>1225</v>
+      </c>
+      <c r="J3" s="1">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1075811</v>
+      </c>
+      <c r="G4" s="2">
+        <v>12095</v>
+      </c>
+      <c r="H4" s="2">
+        <v>8542</v>
+      </c>
+      <c r="I4" s="2">
+        <v>492</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1440</v>
+      </c>
+      <c r="H5" s="1">
+        <v>632</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1440</v>
-      </c>
-      <c r="H4" s="1">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="2">
-        <v>17680</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1542360</v>
-      </c>
-      <c r="G6" s="2">
-        <v>4256</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2">
+        <v>17680</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1542360</v>
+      </c>
+      <c r="G7" s="2">
+        <v>4256</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="2">
-        <v>3852</v>
-      </c>
-      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="G8" s="1">
-        <v>209</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="2">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2">
+        <v>3852</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="1">
+        <v>209</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="2">
         <v>979456</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G10" s="2">
         <v>3644</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H10" s="2">
         <v>1430</v>
+      </c>
+      <c r="I10" s="2">
+        <v>885</v>
+      </c>
+      <c r="J10" s="1">
+        <v>648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes made to the VCF script and added ISSRseq_workflow Gliffy
</commit_message>
<xml_diff>
--- a/development notes/development_run_results.xlsx
+++ b/development notes/development_run_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandon\Documents\ISSRseq\development notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA99404-CAEB-4C2D-BBF7-5F02BF119CEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CD8505-E08D-48C6-850D-146D4CEA0E0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="5760" windowWidth="23310" windowHeight="8355" xr2:uid="{99C3184B-795E-4B96-8633-BF33F0E94C1E}"/>
+    <workbookView xWindow="105" yWindow="990" windowWidth="24780" windowHeight="11835" xr2:uid="{99C3184B-795E-4B96-8633-BF33F0E94C1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Taxon</t>
   </si>
@@ -54,9 +54,6 @@
     <t>pooled PCRs, sheared</t>
   </si>
   <si>
-    <t>variants called</t>
-  </si>
-  <si>
     <t>Populus deltoides</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>STACKS -- pub reported</t>
   </si>
   <si>
-    <t>STACKS -- myco run -- PE</t>
-  </si>
-  <si>
     <t>STACKS -- myco run -- SE</t>
   </si>
   <si>
@@ -120,7 +114,10 @@
     <t>found in 90% of individuals</t>
   </si>
   <si>
-    <t>filtered SNPs</t>
+    <t>GATK-filtered SNPs</t>
+  </si>
+  <si>
+    <t>variants</t>
   </si>
 </sst>
 </file>
@@ -492,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DFE0D0-A0D4-41B8-9114-A09382CB63CC}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,31 +515,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -550,16 +547,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2">
         <v>122941</v>
@@ -582,16 +579,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2">
         <v>1064221</v>
@@ -611,19 +608,19 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="2">
         <v>1075811</v>
@@ -643,22 +640,22 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G5" s="2">
         <v>1440</v>
@@ -667,10 +664,10 @@
         <v>632</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -678,16 +675,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="2">
         <v>17680</v>
@@ -699,82 +696,65 @@
         <v>4256</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2">
+        <v>979456</v>
+      </c>
+      <c r="G8" s="2">
+        <v>3644</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1430</v>
+      </c>
+      <c r="I8" s="2">
+        <v>885</v>
+      </c>
+      <c r="J8" s="1">
+        <v>648</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="2">
         <v>3852</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G9" s="1">
         <v>209</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="2">
-        <v>979456</v>
-      </c>
-      <c r="G10" s="2">
-        <v>3644</v>
-      </c>
-      <c r="H10" s="2">
-        <v>1430</v>
-      </c>
-      <c r="I10" s="2">
-        <v>885</v>
-      </c>
-      <c r="J10" s="1">
-        <v>648</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>